<commit_message>
adding advanced report config
</commit_message>
<xml_diff>
--- a/data/input/portfolios.xlsx
+++ b/data/input/portfolios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caolanraff/Documents/Development/python/git-personal/portfolio-tracker/data/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caolanraff/Documents/Development/python/git-personal/etf-portfolio-tracker/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FCF730-FE60-C64C-9A5A-00AEA00C6B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8BADAD-635D-FB45-8DCC-8FC1CD71777F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>date</t>
   </si>
@@ -72,9 +72,6 @@
     <t>JEPI</t>
   </si>
   <si>
-    <t>SPYW.DE</t>
-  </si>
-  <si>
     <t>CQQQ</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
   </si>
   <si>
     <t>VYMI</t>
-  </si>
-  <si>
-    <t>ISAG.L</t>
   </si>
   <si>
     <t>VSGX</t>
@@ -601,7 +595,9 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -652,7 +648,7 @@
         <v>44927</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C4" s="6">
         <v>1000</v>
@@ -680,7 +676,7 @@
         <v>44927</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="6">
         <v>200</v>
@@ -694,7 +690,7 @@
         <v>44927</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6">
         <v>100</v>
@@ -719,10 +715,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -746,7 +742,7 @@
         <v>44927</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4">
         <v>33</v>
@@ -777,7 +773,7 @@
         <v>44927</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4">
         <v>62</v>
@@ -811,7 +807,7 @@
         <v>44927</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4">
         <v>160</v>
@@ -845,13 +841,13 @@
         <v>44927</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D8" s="4">
-        <v>50.6</v>
+        <v>60.59</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="8"/>
@@ -862,79 +858,68 @@
         <v>44927</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D9" s="4">
-        <v>60.59</v>
-      </c>
-      <c r="G9" s="4"/>
+        <v>48.95</v>
+      </c>
       <c r="H9" s="8"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44927</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="D10" s="4">
-        <v>48.95</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+        <v>56.64</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44927</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D11" s="4">
-        <v>56.64</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+        <v>409.66</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44927</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4">
         <v>25</v>
       </c>
-      <c r="C12" s="4">
-        <v>2</v>
-      </c>
       <c r="D12" s="4">
-        <v>409.66</v>
+        <v>54.27</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>44927</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="4">
-        <v>25</v>
-      </c>
-      <c r="D13" s="4">
-        <v>54.27</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -966,17 +951,11 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>